<commit_message>
Adding new changes to Master
Adding ANA-1061 and ANA-1042 to master along with the changes of methods and objects
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/ANA-1050.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/ANA-1050.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Account</t>
   </si>
@@ -41,12 +41,6 @@
     <t>Component</t>
   </si>
   <si>
-    <t>Order Status</t>
-  </si>
-  <si>
-    <t>Closed On</t>
-  </si>
-  <si>
     <t>InsertCase</t>
   </si>
   <si>
@@ -83,17 +77,35 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Sub Status</t>
-  </si>
-  <si>
     <t>Resolved</t>
+  </si>
+  <si>
+    <t>ClosedOn</t>
+  </si>
+  <si>
+    <t>SubStatus</t>
+  </si>
+  <si>
+    <t>OrderStatus</t>
+  </si>
+  <si>
+    <t>InsertServiceRequest</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Open' );insert SR_1 ;</t>
+  </si>
+  <si>
+    <t>001q000000hmfgo</t>
+  </si>
+  <si>
+    <t>a1Jq0000001faAI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,6 +117,22 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,8 +152,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -139,7 +175,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -430,10 +474,12 @@
     <col min="5" max="5" width="33.6640625" style="1" customWidth="1"/>
     <col min="6" max="8" width="37.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="41.6640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="41.83203125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,57 +493,72 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created the test-case ANA-1053 and updated the sheet of data
Created the test-case ANA-1053 and updated the sheet of data.
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/ANA-1050.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/ANA-1050.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Account</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>a1Jq0000001faAI</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Closed' );insert SR_1 ;</t>
   </si>
 </sst>
 </file>
@@ -152,8 +155,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -175,15 +180,17 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,12 +556,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the test-case ANA-1044.sah.
Adding the test-case ANA-1044.sah and also renaming the suites as per the metrics.
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/ANA-1050.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/ANA-1050.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Account</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Site</t>
   </si>
   <si>
-    <t>001q000000hmXhA</t>
-  </si>
-  <si>
     <t>a1Jq0000001fK4a</t>
   </si>
   <si>
@@ -95,13 +92,22 @@
     <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Open' );insert SR_1 ;</t>
   </si>
   <si>
-    <t>001q000000hmfgo</t>
-  </si>
-  <si>
     <t>a1Jq0000001faAI</t>
   </si>
   <si>
-    <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Closed' );insert SR_1 ;</t>
+    <t>01tq0000001jhI0</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PBEa</t>
+  </si>
+  <si>
+    <t>SVMXC__Service_Request__c SR_1 = new SVMXC__Service_Request__c(SVMXC__Status__c = 'Closed', SVMXC__Priority__c = 'High' );insert SR_1 ;</t>
+  </si>
+  <si>
+    <t>001q000000hmXhAAAU</t>
+  </si>
+  <si>
+    <t>001q000000hmfgoAAA</t>
   </si>
 </sst>
 </file>
@@ -468,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,7 +487,7 @@
     <col min="5" max="5" width="33.6640625" style="1" customWidth="1"/>
     <col min="6" max="8" width="37.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="41.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="20.83203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="41.83203125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -500,16 +506,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -518,49 +524,55 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K3" s="1" t="s">

</xml_diff>